<commit_message>
Fixed deltas.xlsx to new format
</commit_message>
<xml_diff>
--- a/entropy_pooling/deltas.xlsx
+++ b/entropy_pooling/deltas.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ilmari/Documents/OR semma/entropy-poolin/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ilmari/Documents/OR semma/entropy-poolin/entropy_pooling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1317D736-3271-6942-ACD0-D1DE98BEA441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EDC5BD5-B325-0C48-8C15-656A52A93E18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="14940" xr2:uid="{1D3A873C-A6BF-0D40-B6AC-D7CCEE647CA2}"/>
+    <workbookView xWindow="1180" yWindow="1460" windowWidth="27240" windowHeight="14940" xr2:uid="{1D3A873C-A6BF-0D40-B6AC-D7CCEE647CA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +27,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -177,21 +178,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor theme="5"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="4">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -199,52 +194,14 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color theme="5" tint="0.39997558519241921"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="5" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="5" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="5" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="5" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="5" tint="0.39997558519241921"/>
-      </right>
-      <top style="thin">
-        <color theme="5" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="5" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -559,154 +516,673 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89C05325-D792-7F44-AA91-208AF284D800}">
-  <dimension ref="A1:AK5"/>
+  <dimension ref="A1:AK37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AF1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AG1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="AJ1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="AK1" s="3" t="s">
-        <v>35</v>
-      </c>
+    <row r="1" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="1"/>
+      <c r="AD1" s="1"/>
+      <c r="AE1" s="1"/>
+      <c r="AF1" s="1"/>
+      <c r="AG1" s="1"/>
+      <c r="AH1" s="1"/>
+      <c r="AI1" s="1"/>
+      <c r="AJ1" s="1"/>
+      <c r="AK1" s="1"/>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>0.69</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>0.92</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>1.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>0.69</v>
+      </c>
+      <c r="C5">
+        <v>0.92</v>
+      </c>
+      <c r="D5">
+        <v>1.4</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
         <v>1.19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>